<commit_message>
ajout du champs template a liste facture dans apercu
</commit_message>
<xml_diff>
--- a/data/Import/factures.xlsx
+++ b/data/Import/factures.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\animan\Documents\FNE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJET\FNEV4\data\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FC7E6F-401E-405B-953E-15786D37CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="9060" firstSheet="127" activeTab="128"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="117" activeTab="118" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facture comptabilisée N° 556300" sheetId="1" r:id="rId1"/>
@@ -1048,7 +1049,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yy"/>
     <numFmt numFmtId="165" formatCode="0.####"/>
@@ -1397,7 +1398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -1489,7 +1490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1625,7 +1626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1717,7 +1718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1804,7 +1805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6500-000000000000}">
   <dimension ref="A3:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -1919,7 +1920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2011,7 +2012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6700-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2147,7 +2148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6800-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2283,7 +2284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6900-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2354,7 +2355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6A00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2490,7 +2491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2582,7 +2583,7 @@
 </file>
 
 <file path=xl/worksheets/sheet109.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6C00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2713,7 +2714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -2849,7 +2850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet110.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6D00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2985,7 +2986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet111.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3077,7 +3078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet112.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3174,7 +3175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet113.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7000-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3243,7 +3244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3330,7 +3331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7200-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3422,7 +3423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3514,7 +3515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7400-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3583,7 +3584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7500-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3652,11 +3653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3668,7 +3669,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -3744,7 +3745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -3875,7 +3876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet120.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7700-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3962,7 +3963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7800-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4049,7 +4050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7900-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4141,7 +4142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4228,7 +4229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4320,7 +4321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4412,7 +4413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7D00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4504,7 +4505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4596,7 +4597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-7F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4688,10 +4689,10 @@
 </file>
 
 <file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-8000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -4780,7 +4781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -4872,7 +4873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4964,7 +4965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5054,7 +5055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5146,7 +5147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5238,7 +5239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5330,7 +5331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5401,7 +5402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5493,7 +5494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5585,7 +5586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5677,7 +5678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5769,7 +5770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5861,7 +5862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5948,7 +5949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6040,7 +6041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6132,7 +6133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6224,7 +6225,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6314,7 +6315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6406,7 +6407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6498,7 +6499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6590,7 +6591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6682,7 +6683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6751,7 +6752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6843,7 +6844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6935,7 +6936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7068,7 +7069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7160,7 +7161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7252,7 +7253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7388,7 +7389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7480,7 +7481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -7570,7 +7571,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7685,7 +7686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7772,7 +7773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7841,7 +7842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7933,7 +7934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8025,7 +8026,7 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8117,7 +8118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8209,7 +8210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8301,7 +8302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8393,7 +8394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8485,7 +8486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8577,7 +8578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8669,7 +8670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8738,7 +8739,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8835,7 +8836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8927,7 +8928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9019,7 +9020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9111,7 +9112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9203,7 +9204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9290,7 +9291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9382,7 +9383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9474,7 +9475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9566,7 +9567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9658,7 +9659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9794,7 +9795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9886,7 +9887,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9978,7 +9979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10070,7 +10071,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10162,7 +10163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10293,7 +10294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10429,7 +10430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10521,7 +10522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10613,7 +10614,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10705,7 +10706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10774,7 +10775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10866,7 +10867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10958,7 +10959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11050,7 +11051,7 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11186,7 +11187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11278,7 +11279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11370,7 +11371,7 @@
 </file>
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11462,7 +11463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -11598,7 +11599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11685,7 +11686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11821,7 +11822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11913,7 +11914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12005,7 +12006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5100-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12076,7 +12077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12168,7 +12169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5300-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12260,7 +12261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5400-000000000000}">
   <dimension ref="A3:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12331,7 +12332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5500-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12423,7 +12424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5600-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12554,7 +12555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5700-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12646,7 +12647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12782,7 +12783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12918,7 +12919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13054,7 +13055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13146,7 +13147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5B00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13238,7 +13239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5C00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13330,7 +13331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5D00-000000000000}">
   <dimension ref="A3:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13445,7 +13446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5E00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13542,7 +13543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5F00-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13639,7 +13640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6000-000000000000}">
   <dimension ref="A3:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13775,7 +13776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6100-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13867,7 +13868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-6200-000000000000}">
   <dimension ref="A3:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>